<commit_message>
Hardward Interrupts for encoders.
</commit_message>
<xml_diff>
--- a/Termination Schedule.xlsx
+++ b/Termination Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d86598615b1afcf0/Waikato/2022B/ENGEN582/Code/HAS_TelescopeController/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/935963ef373bb62b/src/HAS_TelescopeController/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E7AE1571-FF69-4FC9-AF11-68777254EBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{E7AE1571-FF69-4FC9-AF11-68777254EBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61EFCA11-1A55-48C6-92DA-AA08694553BC}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="300" windowWidth="19543" windowHeight="12137" xr2:uid="{CA35774A-8649-44C4-A98B-AFA17E78A290}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{CA35774A-8649-44C4-A98B-AFA17E78A290}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -513,7 +513,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -920,58 +920,7 @@
         <family val="3"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Inconsolata"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Inconsolata"/>
-        <family val="3"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1010,6 +959,25 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Inconsolata"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1172,6 +1140,38 @@
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Inconsolata"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1185,34 +1185,30 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D0C07187-FF86-4466-8E66-4B6F992F02A6}" name="Table1" displayName="Table1" ref="A2:K44" totalsRowShown="0" headerRowDxfId="0" dataDxfId="13" headerRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D0C07187-FF86-4466-8E66-4B6F992F02A6}" name="Table1" displayName="Table1" ref="A2:K44" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12">
   <autoFilter ref="A2:K44" xr:uid="{D0C07187-FF86-4466-8E66-4B6F992F02A6}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{434384C3-6B87-4173-A4EA-378C2E7043B6}" name="CORE" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{3541E71A-241F-4E96-B678-F2AD4023E4C6}" name="VOLTAGE" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{75F69C94-20BA-44DF-9E10-7EF02B83A123}" name="SOURCE" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{6842CDA9-E51D-4D9F-8187-82D9B8DBC6B8}" name="SOURCE DESCRIPTION" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{21A70157-857B-4A37-9FA4-28E8779CDF9F}" name="SRC TERM" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{8EDECB3D-74AC-4BC5-B574-4BF0BAF809D3}" name="CORE DESCRIPTION" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{2405FE98-B9B1-445F-8915-4162BF245019}" name="FUSE/TERMINAL" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{F282A3D9-291B-4BAA-84CB-00B517E70D64}" name="ENDPOINT" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{655DC419-D1CB-48B9-845F-9ACD77073013}" name="ENDPT DESCRIPTION" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{3DC93154-A17A-40F0-B0CA-A01E0700507F}" name="END TERM" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{A63FC08F-AF8C-4747-96CF-FB7B233FB24C}" name="CABLE" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{434384C3-6B87-4173-A4EA-378C2E7043B6}" name="CORE" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{3541E71A-241F-4E96-B678-F2AD4023E4C6}" name="VOLTAGE" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{75F69C94-20BA-44DF-9E10-7EF02B83A123}" name="SOURCE" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{6842CDA9-E51D-4D9F-8187-82D9B8DBC6B8}" name="SOURCE DESCRIPTION" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{21A70157-857B-4A37-9FA4-28E8779CDF9F}" name="SRC TERM" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{8EDECB3D-74AC-4BC5-B574-4BF0BAF809D3}" name="CORE DESCRIPTION" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{2405FE98-B9B1-445F-8915-4162BF245019}" name="FUSE/TERMINAL" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{F282A3D9-291B-4BAA-84CB-00B517E70D64}" name="ENDPOINT" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{655DC419-D1CB-48B9-845F-9ACD77073013}" name="ENDPT DESCRIPTION" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{3DC93154-A17A-40F0-B0CA-A01E0700507F}" name="END TERM" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{A63FC08F-AF8C-4747-96CF-FB7B233FB24C}" name="CABLE" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1250,7 +1246,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1356,7 +1352,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1498,7 +1494,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1511,27 +1507,27 @@
   </sheetPr>
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.23046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.15234375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="25.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.23046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.69140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.15234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.4609375" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.23046875" style="1"/>
+    <col min="1" max="1" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.42578125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="21">
       <c r="A1" s="34" t="s">
         <v>121</v>
       </c>
@@ -1546,7 +1542,7 @@
       <c r="J1" s="35"/>
       <c r="K1" s="36"/>
     </row>
-    <row r="2" spans="1:11" ht="17.149999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1">
       <c r="A2" s="31" t="s">
         <v>3</v>
       </c>
@@ -1581,7 +1577,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11">
       <c r="A3" s="23">
         <v>10</v>
       </c>
@@ -1608,7 +1604,7 @@
       <c r="J3" s="24"/>
       <c r="K3" s="26"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11">
       <c r="A4" s="4">
         <v>11</v>
       </c>
@@ -1637,7 +1633,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11">
       <c r="A5" s="4">
         <v>12</v>
       </c>
@@ -1664,7 +1660,7 @@
       <c r="J5" s="3"/>
       <c r="K5" s="5"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11">
       <c r="A6" s="4">
         <v>12</v>
       </c>
@@ -1691,7 +1687,7 @@
       <c r="J6" s="3"/>
       <c r="K6" s="5"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11">
       <c r="A7" s="4">
         <v>13</v>
       </c>
@@ -1718,7 +1714,7 @@
       <c r="J7" s="3"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="8" spans="1:11" ht="17.149999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1">
       <c r="A8" s="6">
         <v>14</v>
       </c>
@@ -1745,7 +1741,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" ht="17.149999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" ht="15.75" thickBot="1">
       <c r="A9" s="19">
         <v>20</v>
       </c>
@@ -1776,7 +1772,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11">
       <c r="A10" s="23">
         <v>30</v>
       </c>
@@ -1809,7 +1805,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11">
       <c r="A11" s="4">
         <v>31</v>
       </c>
@@ -1842,7 +1838,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11">
       <c r="A12" s="4">
         <v>32</v>
       </c>
@@ -1875,7 +1871,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11">
       <c r="A13" s="4">
         <v>33</v>
       </c>
@@ -1908,7 +1904,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11">
       <c r="A14" s="4">
         <v>34</v>
       </c>
@@ -1941,7 +1937,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11">
       <c r="A15" s="4">
         <v>35</v>
       </c>
@@ -1974,7 +1970,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11">
       <c r="A16" s="4">
         <v>36</v>
       </c>
@@ -2007,7 +2003,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="17.149999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" ht="15.75" thickBot="1">
       <c r="A17" s="27">
         <v>37</v>
       </c>
@@ -2040,7 +2036,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="17.149999999999999" thickTop="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:11" ht="15.75" thickTop="1">
       <c r="A18" s="4">
         <v>100</v>
       </c>
@@ -2069,7 +2065,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:11">
       <c r="A19" s="4">
         <v>101</v>
       </c>
@@ -2098,7 +2094,7 @@
       </c>
       <c r="K19" s="5"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:11">
       <c r="A20" s="4">
         <v>101</v>
       </c>
@@ -2127,7 +2123,7 @@
       </c>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:11">
       <c r="A21" s="4">
         <v>102</v>
       </c>
@@ -2156,7 +2152,7 @@
       </c>
       <c r="K21" s="5"/>
     </row>
-    <row r="22" spans="1:11" ht="17.149999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" ht="15.75" thickBot="1">
       <c r="A22" s="6">
         <v>103</v>
       </c>
@@ -2179,7 +2175,7 @@
       <c r="J22" s="7"/>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="1:11" ht="17.149999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" ht="15.75" thickBot="1">
       <c r="A23" s="19">
         <v>200</v>
       </c>
@@ -2210,7 +2206,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:11">
       <c r="A24" s="4">
         <v>300</v>
       </c>
@@ -2245,7 +2241,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:11">
       <c r="A25" s="4">
         <v>301</v>
       </c>
@@ -2280,7 +2276,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:11">
       <c r="A26" s="4">
         <v>302</v>
       </c>
@@ -2313,7 +2309,7 @@
       </c>
       <c r="K26" s="5"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:11">
       <c r="A27" s="4">
         <v>303</v>
       </c>
@@ -2346,7 +2342,7 @@
       </c>
       <c r="K27" s="5"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:11">
       <c r="A28" s="4">
         <v>304</v>
       </c>
@@ -2379,7 +2375,7 @@
       </c>
       <c r="K28" s="5"/>
     </row>
-    <row r="29" spans="1:11" ht="17.149999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:11" ht="15.75" thickBot="1">
       <c r="A29" s="11">
         <v>305</v>
       </c>
@@ -2412,7 +2408,7 @@
       </c>
       <c r="K29" s="14"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:11">
       <c r="A30" s="15">
         <v>306</v>
       </c>
@@ -2445,7 +2441,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:11">
       <c r="A31" s="4">
         <v>307</v>
       </c>
@@ -2476,7 +2472,7 @@
       <c r="J31" s="3"/>
       <c r="K31" s="5"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:11">
       <c r="A32" s="4">
         <v>308</v>
       </c>
@@ -2511,7 +2507,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="17.149999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:11" ht="15.75" thickBot="1">
       <c r="A33" s="11">
         <v>309</v>
       </c>
@@ -2546,7 +2542,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:11">
       <c r="A34" s="15">
         <v>310</v>
       </c>
@@ -2581,7 +2577,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:11">
       <c r="A35" s="4">
         <v>311</v>
       </c>
@@ -2616,7 +2612,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:11">
       <c r="A36" s="4">
         <v>312</v>
       </c>
@@ -2651,7 +2647,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="17.149999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:11" ht="15.75" thickBot="1">
       <c r="A37" s="11">
         <v>313</v>
       </c>
@@ -2686,7 +2682,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:11">
       <c r="A38" s="4">
         <v>314</v>
       </c>
@@ -2721,7 +2717,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:11">
       <c r="A39" s="4">
         <v>315</v>
       </c>
@@ -2756,7 +2752,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:11">
       <c r="A40" s="4">
         <v>316</v>
       </c>
@@ -2791,7 +2787,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:11">
       <c r="A41" s="4">
         <v>317</v>
       </c>
@@ -2826,7 +2822,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="17.149999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:11" ht="15.75" thickBot="1">
       <c r="A42" s="11">
         <v>318</v>
       </c>
@@ -2859,7 +2855,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:11">
       <c r="A43" s="4">
         <v>319</v>
       </c>
@@ -2894,7 +2890,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="17.149999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:11" ht="15.75" thickBot="1">
       <c r="A44" s="6">
         <v>320</v>
       </c>
@@ -2935,7 +2931,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="86" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="83" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>

<commit_message>
Added Encoder position. ready to test. Termination schedule updated.
</commit_message>
<xml_diff>
--- a/Termination Schedule.xlsx
+++ b/Termination Schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/935963ef373bb62b/src/HAS_TelescopeController/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{E7AE1571-FF69-4FC9-AF11-68777254EBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61EFCA11-1A55-48C6-92DA-AA08694553BC}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{E7AE1571-FF69-4FC9-AF11-68777254EBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{824A612C-F558-48AA-B5A8-3006379B3830}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{CA35774A-8649-44C4-A98B-AFA17E78A290}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="164">
   <si>
     <t>SOURCE</t>
   </si>
@@ -507,13 +507,34 @@
   </si>
   <si>
     <t>RA Encoder B</t>
+  </si>
+  <si>
+    <t>DI_DEC_ENC_A</t>
+  </si>
+  <si>
+    <t>ENC-01</t>
+  </si>
+  <si>
+    <t>DEC Encoder A</t>
+  </si>
+  <si>
+    <t>A13</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>DI_DEC_ENC_B</t>
+  </si>
+  <si>
+    <t>ENC01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -541,7 +562,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -554,8 +575,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor theme="4" tint="0.59999389629810485"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -784,19 +811,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -897,6 +945,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1122,6 +1182,13 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1139,13 +1206,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1185,21 +1245,25 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D0C07187-FF86-4466-8E66-4B6F992F02A6}" name="Table1" displayName="Table1" ref="A2:K44" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12">
-  <autoFilter ref="A2:K44" xr:uid="{D0C07187-FF86-4466-8E66-4B6F992F02A6}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{007D876F-31F0-4092-8844-CF7C00CA2CD8}" name="Table13" displayName="Table13" ref="A2:K46" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowBorderDxfId="11">
+  <autoFilter ref="A2:K46" xr:uid="{007D876F-31F0-4092-8844-CF7C00CA2CD8}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{434384C3-6B87-4173-A4EA-378C2E7043B6}" name="CORE" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{3541E71A-241F-4E96-B678-F2AD4023E4C6}" name="VOLTAGE" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{75F69C94-20BA-44DF-9E10-7EF02B83A123}" name="SOURCE" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{6842CDA9-E51D-4D9F-8187-82D9B8DBC6B8}" name="SOURCE DESCRIPTION" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{21A70157-857B-4A37-9FA4-28E8779CDF9F}" name="SRC TERM" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{8EDECB3D-74AC-4BC5-B574-4BF0BAF809D3}" name="CORE DESCRIPTION" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{2405FE98-B9B1-445F-8915-4162BF245019}" name="FUSE/TERMINAL" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{F282A3D9-291B-4BAA-84CB-00B517E70D64}" name="ENDPOINT" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{655DC419-D1CB-48B9-845F-9ACD77073013}" name="ENDPT DESCRIPTION" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{3DC93154-A17A-40F0-B0CA-A01E0700507F}" name="END TERM" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{A63FC08F-AF8C-4747-96CF-FB7B233FB24C}" name="CABLE" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{573D4364-1B15-4464-8F37-E5F3ACDE2664}" name="CORE" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{1BE8C6E4-8DC0-4935-B806-E7AE9D714930}" name="VOLTAGE" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{BC8B2989-E894-41E9-9B7D-3EBE630B6A57}" name="SOURCE" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{043EE58B-C57A-4E51-9A79-1A1AFD1CFBDC}" name="SOURCE DESCRIPTION" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{61B76F7C-59A1-4B1B-945B-3AD5EEE55261}" name="SRC TERM" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{1D30B743-40C9-4B09-98C1-52A2A1387844}" name="CORE DESCRIPTION" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{EE120C4F-7396-4890-90A4-F1F1B3DBD1EC}" name="FUSE/TERMINAL" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{1B320576-DBFF-409E-ADAA-6DE0FD928E45}" name="ENDPOINT" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{89280C9E-38A7-4C0A-BEFF-76F0979447F6}" name="ENDPT DESCRIPTION" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{07C978E2-27AA-4774-A7F9-2BB8D99B122A}" name="END TERM" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{62F99B1F-3CA2-47C1-BB5C-BC74EE0F4B86}" name="CABLE" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1505,13 +1569,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.140625" style="1" bestFit="1" customWidth="1"/>
@@ -1527,1402 +1591,1452 @@
     <col min="12" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="36"/>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A2" s="31" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="35"/>
+    </row>
+    <row r="2" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="32" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="23">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="22">
         <v>10</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24" t="s">
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="24"/>
-      <c r="K3" s="26"/>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="4">
+      <c r="J3" s="23"/>
+      <c r="K3" s="25"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="3" t="s">
+      <c r="E4" s="2"/>
+      <c r="G4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="5" t="s">
+      <c r="J4" s="2"/>
+      <c r="K4" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5" s="4">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="3" t="s">
+      <c r="E5" s="2"/>
+      <c r="G5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="H5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="K5" s="5"/>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="4">
+      <c r="J5" s="2"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>12</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="3" t="s">
+      <c r="E6" s="2"/>
+      <c r="G6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="5"/>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="4">
+      <c r="J6" s="2"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>13</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="3" t="s">
+      <c r="E7" s="2"/>
+      <c r="G7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="K7" s="5"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A8" s="6">
+      <c r="J7" s="2"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5">
         <v>14</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="7" t="s">
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="7"/>
-      <c r="K8" s="10"/>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A9" s="19">
+      <c r="J8" s="6"/>
+      <c r="K8" s="9"/>
+    </row>
+    <row r="9" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="18">
         <v>20</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="20" t="s">
+      <c r="E9" s="19"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="21" t="s">
+      <c r="I9" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="20" t="s">
+      <c r="J9" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="22" t="s">
+      <c r="K9" s="21" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="23">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="22">
         <v>30</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="25"/>
-      <c r="G10" s="24" t="s">
+      <c r="F10" s="24"/>
+      <c r="G10" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="23" t="s">
         <v>149</v>
       </c>
-      <c r="I10" s="25" t="s">
+      <c r="I10" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="24" t="s">
+      <c r="J10" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="26" t="s">
+      <c r="K10" s="25" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="4">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>31</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="J11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="4">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>32</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="4">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
         <v>33</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="J13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="5" t="s">
+      <c r="K13" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="4">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
         <v>34</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="J14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="K14" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="4">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
         <v>35</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="J15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="K15" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="4">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
         <v>36</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="H16" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="J16" s="3" t="s">
+      <c r="J16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="K16" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A17" s="27">
+    <row r="17" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="26">
         <v>37</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="29"/>
-      <c r="G17" s="28" t="s">
+      <c r="F17" s="28"/>
+      <c r="G17" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="28" t="s">
+      <c r="H17" s="27" t="s">
         <v>150</v>
       </c>
-      <c r="I17" s="29" t="s">
+      <c r="I17" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="J17" s="28" t="s">
+      <c r="J17" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="K17" s="30" t="s">
+      <c r="K17" s="29" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15.75" thickTop="1">
-      <c r="A18" s="4">
+    <row r="18" spans="1:11" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
         <v>100</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3" t="s">
+      <c r="E18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="3" t="s">
+      <c r="J18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="K18" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="4">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>101</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="3" t="s">
+      <c r="E19" s="2"/>
+      <c r="G19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="J19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K19" s="5"/>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="4">
+      <c r="K19" s="4"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
         <v>101</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="3" t="s">
+      <c r="E20" s="2"/>
+      <c r="G20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J20" s="3" t="s">
+      <c r="J20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K20" s="5"/>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="4">
+      <c r="K20" s="4"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
         <v>102</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="3" t="s">
+      <c r="E21" s="2"/>
+      <c r="G21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="H21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="I21" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="J21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K21" s="5"/>
-    </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A22" s="6">
+      <c r="K21" s="4"/>
+    </row>
+    <row r="22" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
         <v>103</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="7"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="8" t="s">
+      <c r="E22" s="6"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="J22" s="7"/>
-      <c r="K22" s="10"/>
-    </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A23" s="19">
+      <c r="J22" s="6"/>
+      <c r="K22" s="9"/>
+    </row>
+    <row r="23" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="18">
         <v>200</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="D23" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="21"/>
-      <c r="G23" s="20" t="s">
+      <c r="E23" s="19"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="H23" s="20" t="s">
+      <c r="H23" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="I23" s="21" t="s">
+      <c r="I23" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="J23" s="20" t="s">
+      <c r="J23" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="K23" s="22" t="s">
+      <c r="K23" s="21" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="4">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>319</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E24" s="2">
+        <v>2</v>
+      </c>
+      <c r="F24" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="I24" s="36" t="s">
+        <v>155</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>320</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="2">
+        <v>3</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="I25" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>302</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E26" s="2">
+        <v>4</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="K26" s="4"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>303</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E27" s="2">
+        <v>5</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="K27" s="4"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>304</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E28" s="2">
+        <v>6</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="10">
+        <v>305</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" s="11">
+        <v>7</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="J29" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="K29" s="13"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="14">
+        <v>306</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E30" s="15">
+        <v>8</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H30" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="J30" s="15"/>
+      <c r="K30" s="17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>307</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="2">
+        <v>9</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="J31" s="2"/>
+      <c r="K31" s="4"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>308</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="2">
+        <v>11</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="10">
+        <v>309</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E33" s="11">
+        <v>12</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="I33" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="J33" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="K33" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="14">
+        <v>310</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" s="15">
+        <v>18</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="G34" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H34" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I34" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J34" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="K34" s="17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>311</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E35" s="2">
+        <v>19</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="K35" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>312</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E36" s="2">
+        <v>20</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="10">
+        <v>313</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E37" s="11">
+        <v>21</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="J37" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="K37" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>314</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>315</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>316</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>317</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="J41" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="10">
+        <v>318</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="D42" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="H42" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="I42" s="12"/>
+      <c r="J42" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="K42" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
         <v>300</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C43" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D43" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E24" s="3">
-        <v>2</v>
-      </c>
-      <c r="F24" s="2" t="s">
+      <c r="E43" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="5">
+        <v>320</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="K44" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>301</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E45" s="38" t="s">
+        <v>160</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H24" s="3" t="s">
+      <c r="G45" s="2"/>
+      <c r="H45" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J24" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="K24" s="5" t="s">
+      <c r="I45" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="K45" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="4">
-        <v>301</v>
-      </c>
-      <c r="B25" s="3" t="s">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+      <c r="B46" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C46" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D46" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E25" s="3">
-        <v>3</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="K25" s="5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="4">
-        <v>302</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E26" s="3">
-        <v>4</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="K26" s="5"/>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="4">
-        <v>303</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E27" s="3">
-        <v>5</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="J27" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="K27" s="5"/>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="4">
-        <v>304</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E28" s="3">
-        <v>6</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="J28" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="K28" s="5"/>
-    </row>
-    <row r="29" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A29" s="11">
-        <v>305</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E29" s="12">
-        <v>7</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="G29" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="H29" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="I29" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="J29" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="K29" s="14"/>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="15">
-        <v>306</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E30" s="16">
-        <v>8</v>
-      </c>
-      <c r="F30" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="G30" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="H30" s="16" t="s">
-        <v>151</v>
-      </c>
-      <c r="I30" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="J30" s="16"/>
-      <c r="K30" s="18" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" s="4">
-        <v>307</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E31" s="3">
-        <v>9</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="J31" s="3"/>
-      <c r="K31" s="5"/>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" s="4">
-        <v>308</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E32" s="3">
-        <v>11</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="K32" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A33" s="11">
-        <v>309</v>
-      </c>
-      <c r="B33" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D33" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E33" s="12">
-        <v>12</v>
-      </c>
-      <c r="F33" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="G33" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="H33" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="I33" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="J33" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="K33" s="14" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
-      <c r="A34" s="15">
-        <v>310</v>
-      </c>
-      <c r="B34" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C34" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E34" s="16">
-        <v>18</v>
-      </c>
-      <c r="F34" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="G34" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H34" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="I34" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="J34" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="K34" s="18" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="A35" s="4">
-        <v>311</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E35" s="3">
-        <v>19</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="J35" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
-      <c r="A36" s="4">
-        <v>312</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E36" s="3">
-        <v>20</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="H36" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="J36" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A37" s="11">
-        <v>313</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E37" s="12">
-        <v>21</v>
-      </c>
-      <c r="F37" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="G37" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="H37" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="I37" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="J37" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="K37" s="14" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11">
-      <c r="A38" s="4">
-        <v>314</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="K38" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11">
-      <c r="A39" s="4">
-        <v>315</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="J39" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="K39" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11">
-      <c r="A40" s="4">
-        <v>316</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="J40" s="3" t="s">
+      <c r="E46" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="F46" s="39" t="s">
+        <v>162</v>
+      </c>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="J46" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="K40" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11">
-      <c r="A41" s="4">
-        <v>317</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="J41" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="K41" s="5" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A42" s="11">
-        <v>318</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="F42" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="G42" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="H42" s="12" t="s">
-        <v>153</v>
-      </c>
-      <c r="I42" s="13"/>
-      <c r="J42" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="K42" s="14" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
-      <c r="A43" s="4">
-        <v>319</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="J43" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="K43" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A44" s="6">
-        <v>320</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H44" s="7" t="s">
-        <v>154</v>
-      </c>
-      <c r="I44" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="J44" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="K44" s="10" t="s">
-        <v>104</v>
+      <c r="K46" s="4" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Wiring Termination documentation.
</commit_message>
<xml_diff>
--- a/Termination Schedule.xlsx
+++ b/Termination Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/935963ef373bb62b/src/HAS_TelescopeController/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{E7AE1571-FF69-4FC9-AF11-68777254EBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{824A612C-F558-48AA-B5A8-3006379B3830}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="8_{E7AE1571-FF69-4FC9-AF11-68777254EBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{426068ED-5DE6-4082-9A43-89662F77C4D7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{CA35774A-8649-44C4-A98B-AFA17E78A290}"/>
   </bookViews>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="165">
   <si>
     <t>SOURCE</t>
   </si>
@@ -528,6 +526,9 @@
   </si>
   <si>
     <t>ENC01</t>
+  </si>
+  <si>
+    <t>DEC Encoder B</t>
   </si>
 </sst>
 </file>
@@ -562,7 +563,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -581,8 +582,32 @@
         <bgColor theme="4" tint="0.59999389629810485"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="24">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -702,17 +727,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="mediumDashed">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -726,17 +740,6 @@
     <border>
       <left/>
       <right/>
-      <top style="mediumDashed">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="mediumDashed">
         <color indexed="64"/>
       </top>
@@ -835,11 +838,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -883,58 +901,64 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -946,17 +970,20 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1182,13 +1209,6 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1206,6 +1226,13 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1250,7 +1277,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{007D876F-31F0-4092-8844-CF7C00CA2CD8}" name="Table13" displayName="Table13" ref="A2:K46" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{007D876F-31F0-4092-8844-CF7C00CA2CD8}" name="Table13" displayName="Table13" ref="A2:K46" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12">
   <autoFilter ref="A2:K46" xr:uid="{007D876F-31F0-4092-8844-CF7C00CA2CD8}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{573D4364-1B15-4464-8F37-E5F3ACDE2664}" name="CORE" dataDxfId="10"/>
@@ -1569,10 +1596,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K46"/>
+  <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="17.25" x14ac:dyDescent="0.25"/>
@@ -1588,85 +1615,86 @@
     <col min="9" max="9" width="36.42578125" style="1" customWidth="1"/>
     <col min="10" max="10" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.42578125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.28515625" style="1"/>
+    <col min="12" max="12" width="3.5703125" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="37"/>
     </row>
     <row r="2" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="31" t="s">
+      <c r="J2" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="30" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="22">
+      <c r="A3" s="20">
         <v>10</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23" t="s">
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="23"/>
-      <c r="K3" s="25"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="23"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -1802,66 +1830,66 @@
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18">
+      <c r="A9" s="16">
         <v>20</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="19" t="s">
+      <c r="E9" s="17"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="H9" s="19" t="s">
+      <c r="H9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="I9" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="19" t="s">
+      <c r="J9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="K9" s="21" t="s">
+      <c r="K9" s="19" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="22">
+      <c r="A10" s="20">
         <v>30</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="23" t="s">
+      <c r="F10" s="22"/>
+      <c r="G10" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="23" t="s">
+      <c r="H10" s="21" t="s">
         <v>149</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="J10" s="23" t="s">
+      <c r="J10" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="25" t="s">
+      <c r="K10" s="23" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2057,40 +2085,40 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26">
+    <row r="17" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="24">
         <v>37</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="27" t="s">
+      <c r="E17" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="27" t="s">
+      <c r="F17" s="26"/>
+      <c r="G17" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="27" t="s">
+      <c r="H17" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="I17" s="28" t="s">
+      <c r="I17" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="J17" s="27" t="s">
+      <c r="J17" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="K17" s="29" t="s">
+      <c r="K17" s="27" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="18" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>100</v>
       </c>
@@ -2118,7 +2146,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>101</v>
       </c>
@@ -2146,7 +2174,7 @@
       </c>
       <c r="K19" s="4"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>101</v>
       </c>
@@ -2174,7 +2202,7 @@
       </c>
       <c r="K20" s="4"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>102</v>
       </c>
@@ -2202,7 +2230,7 @@
       </c>
       <c r="K21" s="4"/>
     </row>
-    <row r="22" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <v>103</v>
       </c>
@@ -2225,38 +2253,38 @@
       <c r="J22" s="6"/>
       <c r="K22" s="9"/>
     </row>
-    <row r="23" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="18">
+    <row r="23" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="16">
         <v>200</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="19"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="19" t="s">
+      <c r="E23" s="17"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="H23" s="19" t="s">
+      <c r="H23" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="I23" s="20" t="s">
+      <c r="I23" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="J23" s="19" t="s">
+      <c r="J23" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="K23" s="21" t="s">
+      <c r="K23" s="19" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>319</v>
       </c>
@@ -2272,7 +2300,7 @@
       <c r="E24" s="2">
         <v>2</v>
       </c>
-      <c r="F24" s="36" t="s">
+      <c r="F24" s="31" t="s">
         <v>94</v>
       </c>
       <c r="G24" s="2" t="s">
@@ -2281,17 +2309,18 @@
       <c r="H24" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I24" s="36" t="s">
+      <c r="I24" s="31" t="s">
         <v>155</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="K24" s="4" t="s">
+      <c r="K24" s="38" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="39"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>320</v>
       </c>
@@ -2307,7 +2336,7 @@
       <c r="E25" s="2">
         <v>3</v>
       </c>
-      <c r="F25" s="37" t="s">
+      <c r="F25" s="32" t="s">
         <v>157</v>
       </c>
       <c r="G25" s="2" t="s">
@@ -2316,7 +2345,7 @@
       <c r="H25" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="I25" s="36" t="s">
+      <c r="I25" s="31" t="s">
         <v>159</v>
       </c>
       <c r="J25" s="2" t="s">
@@ -2325,8 +2354,9 @@
       <c r="K25" s="2" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="39"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>302</v>
       </c>
@@ -2357,9 +2387,10 @@
       <c r="J26" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="K26" s="4"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K26" s="38"/>
+      <c r="L26" s="40"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>303</v>
       </c>
@@ -2390,9 +2421,10 @@
       <c r="J27" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="K27" s="4"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K27" s="38"/>
+      <c r="L27" s="40"/>
+    </row>
+    <row r="28" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>304</v>
       </c>
@@ -2417,15 +2449,16 @@
       <c r="H28" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>110</v>
+      <c r="I28" s="12" t="s">
+        <v>111</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="K28" s="4"/>
-    </row>
-    <row r="29" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K28" s="38"/>
+      <c r="L28" s="40"/>
+    </row>
+    <row r="29" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10">
         <v>305</v>
       </c>
@@ -2450,48 +2483,50 @@
       <c r="H29" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I29" s="12" t="s">
-        <v>111</v>
+      <c r="I29" s="1" t="s">
+        <v>110</v>
       </c>
       <c r="J29" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="K29" s="13"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="14">
+      <c r="K29" s="11"/>
+      <c r="L29" s="40"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="13">
         <v>306</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E30" s="15">
+      <c r="E30" s="14">
         <v>8</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="F30" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G30" s="15" t="s">
+      <c r="G30" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="H30" s="15" t="s">
+      <c r="H30" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="I30" s="16" t="s">
+      <c r="I30" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="J30" s="15"/>
-      <c r="K30" s="17" t="s">
+      <c r="J30" s="14"/>
+      <c r="K30" s="14" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" s="41"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>307</v>
       </c>
@@ -2520,9 +2555,10 @@
         <v>113</v>
       </c>
       <c r="J31" s="2"/>
-      <c r="K31" s="4"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K31" s="38"/>
+      <c r="L31" s="41"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>308</v>
       </c>
@@ -2553,11 +2589,12 @@
       <c r="J32" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="K32" s="4" t="s">
+      <c r="K32" s="38" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L32" s="42"/>
+    </row>
+    <row r="33" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10">
         <v>309</v>
       </c>
@@ -2588,46 +2625,48 @@
       <c r="J33" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="K33" s="13" t="s">
+      <c r="K33" s="11" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="14">
+      <c r="L33" s="42"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="13">
         <v>310</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C34" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E34" s="15">
+      <c r="E34" s="14">
         <v>18</v>
       </c>
-      <c r="F34" s="16" t="s">
+      <c r="F34" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="G34" s="15" t="s">
+      <c r="G34" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="H34" s="15" t="s">
+      <c r="H34" s="14" t="s">
         <v>153</v>
       </c>
-      <c r="I34" s="16" t="s">
+      <c r="I34" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="J34" s="15" t="s">
+      <c r="J34" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="K34" s="17" t="s">
+      <c r="K34" s="14" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34" s="42"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>311</v>
       </c>
@@ -2658,11 +2697,12 @@
       <c r="J35" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="K35" s="4" t="s">
+      <c r="K35" s="38" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35" s="42"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>312</v>
       </c>
@@ -2693,11 +2733,12 @@
       <c r="J36" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="K36" s="4" t="s">
+      <c r="K36" s="38" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L36" s="42"/>
+    </row>
+    <row r="37" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10">
         <v>313</v>
       </c>
@@ -2728,11 +2769,12 @@
       <c r="J37" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="K37" s="13" t="s">
+      <c r="K37" s="11" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L37" s="42"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>314</v>
       </c>
@@ -2763,11 +2805,12 @@
       <c r="J38" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="K38" s="4" t="s">
+      <c r="K38" s="38" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L38" s="42"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>315</v>
       </c>
@@ -2798,11 +2841,12 @@
       <c r="J39" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="K39" s="4" t="s">
+      <c r="K39" s="38" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L39" s="42"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>316</v>
       </c>
@@ -2833,11 +2877,12 @@
       <c r="J40" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="K40" s="4" t="s">
+      <c r="K40" s="38" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40" s="42"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>317</v>
       </c>
@@ -2868,11 +2913,12 @@
       <c r="J41" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="K41" s="4" t="s">
+      <c r="K41" s="38" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L41" s="42"/>
+    </row>
+    <row r="42" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10">
         <v>318</v>
       </c>
@@ -2901,11 +2947,12 @@
       <c r="J42" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="K42" s="13" t="s">
+      <c r="K42" s="11" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L42" s="42"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>300</v>
       </c>
@@ -2936,11 +2983,12 @@
       <c r="J43" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="K43" s="4" t="s">
+      <c r="K43" s="38" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L43" s="41"/>
+    </row>
+    <row r="44" spans="1:12" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>320</v>
       </c>
@@ -2971,11 +3019,12 @@
       <c r="J44" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="K44" s="9" t="s">
+      <c r="K44" s="6" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L44" s="39"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>301</v>
       </c>
@@ -2988,7 +3037,7 @@
       <c r="D45" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E45" s="38" t="s">
+      <c r="E45" s="33" t="s">
         <v>160</v>
       </c>
       <c r="F45" s="1" t="s">
@@ -3004,12 +3053,15 @@
       <c r="J45" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="K45" s="4" t="s">
+      <c r="K45" s="38" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="3"/>
+      <c r="L45" s="41"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>321</v>
+      </c>
       <c r="B46" s="2" t="s">
         <v>6</v>
       </c>
@@ -3019,10 +3071,10 @@
       <c r="D46" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E46" s="38" t="s">
+      <c r="E46" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="F46" s="39" t="s">
+      <c r="F46" s="34" t="s">
         <v>162</v>
       </c>
       <c r="G46" s="2"/>
@@ -3030,14 +3082,15 @@
         <v>163</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="J46" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="K46" s="4" t="s">
+      <c r="K46" s="38" t="s">
         <v>158</v>
       </c>
+      <c r="L46" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3045,7 +3098,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="83" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="82" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>